<commit_message>
Atualização automática de OSORIO.xlsx
</commit_message>
<xml_diff>
--- a/OSORIO.xlsx
+++ b/OSORIO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{38A90F2E-F2AD-4D4E-AD99-7B71EBCE1978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{13B43FA4-404A-4C87-8384-D29C082BF4DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,20 +22,7 @@
     <sheet name="Recolhimento x Eliminacao" sheetId="6" r:id="rId7"/>
     <sheet name="Desarquivamentos Pendentes" sheetId="7" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -1225,7 +1212,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1285,36 +1272,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1353,14 +1316,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1414,7 +1372,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{1B8CFC31-94B3-41DF-8006-9CBE17663F35}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{25F21AD0-71FC-46D7-9139-F4D7110371F5}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1444,10 +1402,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6946D0F4-4BBE-4276-9887-D30AE2C7CACF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF60AC2F-9A02-4BC6-A5D6-81220E080F59}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1485,7 +1443,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83EA5604-D5E7-4D31-9F67-35E49CD954B7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE771099-84BF-4EAD-8926-7F33F12E7445}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1548,7 +1506,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC0EC963-720F-48D6-B588-725BB53751BA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2CA2BAE5-B5EB-4E4D-8182-1964AFE17143}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1567,7 +1525,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE05F932-A4AF-DCC7-2DD6-16EEB44D5FA2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{22272242-BF9C-34AA-844C-5E1939D9AB6A}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1616,7 +1574,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D7738AA-871C-DE40-DC57-E06AF5AB77A2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{683F0F97-6159-06CC-8385-7652DB4546CE}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1635,7 +1593,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C273F55D-6F8A-C87A-4C6D-31465786518B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E96FA8D-47EE-4CE7-2E8A-450C988CD8DF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1666,7 +1624,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EEBDBAF-C21B-512C-9085-82E926146727}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BF544BA-908F-AF8A-D37D-46165E832B40}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1697,7 +1655,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2ABF4743-8687-8E0B-E237-9AEAA3137330}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8FF8879E-F3F2-632E-C262-11E8E2C976C9}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1740,7 +1698,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BDFCAE54-4799-454D-9F30-4A7BDBD0B424}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E62E9086-5F25-4175-A2E1-57DDFC35FC26}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1778,7 +1736,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9CF1A33F-B338-4A81-A7D1-BDA387E1984B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD034A73-7AA4-4492-ABC8-F4A149B36337}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1821,7 +1779,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D144B69-DC03-4023-9571-8F975703EAD5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A0B7F5E-2691-4206-BFD3-D4CD6D103A1C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2134,7 +2092,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60749E64-C3EE-4EFB-B907-819CBD5DD8B6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D2E3BE7-9334-4A0D-90E6-BCD3DD4771F3}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2146,98 +2104,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="41"/>
-    <col min="6" max="6" width="2" style="41" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="41" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="41"/>
+    <col min="1" max="5" width="12.5703125" style="38"/>
+    <col min="6" max="6" width="2" style="38" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="38" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="40"/>
+      <c r="F1" s="37"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="40"/>
+      <c r="F2" s="37"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="40"/>
+      <c r="F3" s="37"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="40"/>
+      <c r="F4" s="37"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="40"/>
+      <c r="F5" s="37"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="40"/>
+      <c r="F6" s="37"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="40"/>
+      <c r="F7" s="37"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="40"/>
+      <c r="F8" s="37"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="40"/>
+      <c r="F9" s="37"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="40"/>
+      <c r="F10" s="37"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="40"/>
+      <c r="F11" s="37"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="40"/>
+      <c r="F12" s="37"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="40"/>
+      <c r="F13" s="37"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="40"/>
+      <c r="F14" s="37"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="40"/>
+      <c r="F15" s="37"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="40"/>
+      <c r="F16" s="37"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="40"/>
+      <c r="F17" s="37"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="40"/>
+      <c r="F18" s="37"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="40"/>
+      <c r="F19" s="37"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="40"/>
+      <c r="F20" s="37"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="40"/>
+      <c r="F21" s="37"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="40"/>
+      <c r="F22" s="37"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="40"/>
+      <c r="F23" s="37"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="40"/>
+      <c r="F24" s="37"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="40"/>
+      <c r="F25" s="37"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="40"/>
+      <c r="F26" s="37"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="40"/>
+      <c r="F27" s="37"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="40"/>
+      <c r="F28" s="37"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="40"/>
+      <c r="F29" s="37"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5473,19 +5431,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>270</v>
       </c>
     </row>
@@ -5508,79 +5466,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>271</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="20" t="s">
         <v>275</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="20" t="s">
         <v>277</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="19" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="20" t="s">
         <v>278</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="19" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="20" t="s">
         <v>279</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="19" t="s">
         <v>274</v>
       </c>
     </row>
@@ -5598,16 +5556,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="89" customWidth="1"/>
+    <col min="10" max="10" width="72.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5641,7 +5599,7 @@
       <c r="J1" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="21" t="s">
         <v>289</v>
       </c>
     </row>
@@ -5655,10 +5613,10 @@
       <c r="C2" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="22">
         <v>78.900000000000006</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="22">
         <v>7.89</v>
       </c>
       <c r="F2" s="2">
@@ -5676,7 +5634,7 @@
       <c r="J2" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K2" s="26">
+      <c r="K2" s="23">
         <v>588</v>
       </c>
     </row>
@@ -5690,10 +5648,10 @@
       <c r="C3" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="D3" s="25">
+      <c r="D3" s="22">
         <v>78.900000000000006</v>
       </c>
-      <c r="E3" s="25">
+      <c r="E3" s="22">
         <v>7.89</v>
       </c>
       <c r="F3" s="2">
@@ -5711,7 +5669,7 @@
       <c r="J3" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K3" s="26">
+      <c r="K3" s="23">
         <v>588</v>
       </c>
     </row>
@@ -5725,10 +5683,10 @@
       <c r="C4" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="D4" s="25">
+      <c r="D4" s="22">
         <v>78.900000000000006</v>
       </c>
-      <c r="E4" s="25">
+      <c r="E4" s="22">
         <v>7.89</v>
       </c>
       <c r="F4" s="2">
@@ -5746,7 +5704,7 @@
       <c r="J4" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K4" s="26">
+      <c r="K4" s="23">
         <v>588</v>
       </c>
     </row>
@@ -5760,10 +5718,10 @@
       <c r="C5" s="2" t="s">
         <v>296</v>
       </c>
-      <c r="D5" s="25">
+      <c r="D5" s="22">
         <v>78.900000000000006</v>
       </c>
-      <c r="E5" s="25">
+      <c r="E5" s="22">
         <v>7.89</v>
       </c>
       <c r="F5" s="2">
@@ -5781,7 +5739,7 @@
       <c r="J5" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K5" s="26">
+      <c r="K5" s="23">
         <v>9865</v>
       </c>
     </row>
@@ -5795,10 +5753,10 @@
       <c r="C6" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="22">
         <v>78.900000000000006</v>
       </c>
-      <c r="E6" s="25">
+      <c r="E6" s="22">
         <v>7.89</v>
       </c>
       <c r="F6" s="2">
@@ -5816,7 +5774,7 @@
       <c r="J6" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K6" s="26">
+      <c r="K6" s="23">
         <v>588</v>
       </c>
     </row>
@@ -5830,10 +5788,10 @@
       <c r="C7" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="D7" s="25">
+      <c r="D7" s="22">
         <v>78.900000000000006</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="22">
         <v>7.89</v>
       </c>
       <c r="F7" s="2">
@@ -5851,7 +5809,7 @@
       <c r="J7" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K7" s="26">
+      <c r="K7" s="23">
         <v>588</v>
       </c>
     </row>
@@ -5865,10 +5823,10 @@
       <c r="C8" s="2" t="s">
         <v>299</v>
       </c>
-      <c r="D8" s="25">
+      <c r="D8" s="22">
         <v>116.2</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="22">
         <v>11.62</v>
       </c>
       <c r="F8" s="2">
@@ -5886,7 +5844,7 @@
       <c r="J8" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K8" s="26">
+      <c r="K8" s="23">
         <v>588</v>
       </c>
     </row>
@@ -5900,10 +5858,10 @@
       <c r="C9" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D9" s="25">
+      <c r="D9" s="22">
         <v>898</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="22">
         <v>89.8</v>
       </c>
       <c r="F9" s="2">
@@ -5921,7 +5879,7 @@
       <c r="J9" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K9" s="26">
+      <c r="K9" s="23">
         <v>588</v>
       </c>
     </row>
@@ -5935,10 +5893,10 @@
       <c r="C10" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D10" s="25">
+      <c r="D10" s="22">
         <v>1495</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="22">
         <v>149.5</v>
       </c>
       <c r="F10" s="2">
@@ -5956,7 +5914,7 @@
       <c r="J10" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K10" s="26">
+      <c r="K10" s="23">
         <v>588</v>
       </c>
     </row>
@@ -5970,10 +5928,10 @@
       <c r="C11" s="2" t="s">
         <v>302</v>
       </c>
-      <c r="D11" s="25">
+      <c r="D11" s="22">
         <v>297</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="22">
         <v>29.7</v>
       </c>
       <c r="F11" s="2">
@@ -5991,7 +5949,7 @@
       <c r="J11" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K11" s="26">
+      <c r="K11" s="23">
         <v>588</v>
       </c>
     </row>
@@ -6005,10 +5963,10 @@
       <c r="C12" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="D12" s="25">
+      <c r="D12" s="22">
         <v>2113.4</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="22">
         <v>422.68</v>
       </c>
       <c r="F12" s="2">
@@ -6026,7 +5984,7 @@
       <c r="J12" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K12" s="26">
+      <c r="K12" s="23">
         <v>156</v>
       </c>
     </row>
@@ -6040,10 +5998,10 @@
       <c r="C13" s="2" t="s">
         <v>305</v>
       </c>
-      <c r="D13" s="25">
+      <c r="D13" s="22">
         <v>36</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="22">
         <v>3.6</v>
       </c>
       <c r="F13" s="2">
@@ -6061,7 +6019,7 @@
       <c r="J13" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K13" s="26">
+      <c r="K13" s="23">
         <v>588</v>
       </c>
     </row>
@@ -6075,10 +6033,10 @@
       <c r="C14" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D14" s="25">
+      <c r="D14" s="22">
         <v>70.95</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="22">
         <v>7.1</v>
       </c>
       <c r="F14" s="2">
@@ -6096,7 +6054,7 @@
       <c r="J14" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K14" s="26">
+      <c r="K14" s="23">
         <v>10030</v>
       </c>
     </row>
@@ -6110,10 +6068,10 @@
       <c r="C15" s="2" t="s">
         <v>309</v>
       </c>
-      <c r="D15" s="25">
+      <c r="D15" s="22">
         <v>75.900000000000006</v>
       </c>
-      <c r="E15" s="25">
+      <c r="E15" s="22">
         <v>7.59</v>
       </c>
       <c r="F15" s="2">
@@ -6131,7 +6089,7 @@
       <c r="J15" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K15" s="26">
+      <c r="K15" s="23">
         <v>9865</v>
       </c>
     </row>
@@ -6145,10 +6103,10 @@
       <c r="C16" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="D16" s="25">
+      <c r="D16" s="22">
         <v>132</v>
       </c>
-      <c r="E16" s="25">
+      <c r="E16" s="22">
         <v>13.2</v>
       </c>
       <c r="F16" s="2">
@@ -6166,7 +6124,7 @@
       <c r="J16" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="K16" s="26">
+      <c r="K16" s="23">
         <v>9357</v>
       </c>
     </row>
@@ -6180,10 +6138,10 @@
       <c r="C17" s="2" t="s">
         <v>312</v>
       </c>
-      <c r="D17" s="25">
+      <c r="D17" s="22">
         <v>144</v>
       </c>
-      <c r="E17" s="25">
+      <c r="E17" s="22">
         <v>14.4</v>
       </c>
       <c r="F17" s="2">
@@ -6201,7 +6159,7 @@
       <c r="J17" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K17" s="26">
+      <c r="K17" s="23">
         <v>588</v>
       </c>
     </row>
@@ -6215,10 +6173,10 @@
       <c r="C18" s="2" t="s">
         <v>313</v>
       </c>
-      <c r="D18" s="25">
+      <c r="D18" s="22">
         <v>665</v>
       </c>
-      <c r="E18" s="25">
+      <c r="E18" s="22">
         <v>133</v>
       </c>
       <c r="F18" s="2">
@@ -6236,7 +6194,7 @@
       <c r="J18" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K18" s="26">
+      <c r="K18" s="23">
         <v>156</v>
       </c>
     </row>
@@ -6250,10 +6208,10 @@
       <c r="C19" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="D19" s="25">
+      <c r="D19" s="22">
         <v>1186</v>
       </c>
-      <c r="E19" s="25">
+      <c r="E19" s="22">
         <v>118.6</v>
       </c>
       <c r="F19" s="2">
@@ -6271,7 +6229,7 @@
       <c r="J19" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="K19" s="26">
+      <c r="K19" s="23">
         <v>17471</v>
       </c>
     </row>
@@ -6285,10 +6243,10 @@
       <c r="C20" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="D20" s="25">
+      <c r="D20" s="22">
         <v>390</v>
       </c>
-      <c r="E20" s="25">
+      <c r="E20" s="22">
         <v>39</v>
       </c>
       <c r="F20" s="2">
@@ -6306,7 +6264,7 @@
       <c r="J20" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K20" s="26">
+      <c r="K20" s="23">
         <v>9865</v>
       </c>
     </row>
@@ -6320,10 +6278,10 @@
       <c r="C21" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="D21" s="25">
+      <c r="D21" s="22">
         <v>4457</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="22">
         <v>445.7</v>
       </c>
       <c r="F21" s="2">
@@ -6341,7 +6299,7 @@
       <c r="J21" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="K21" s="26">
+      <c r="K21" s="23">
         <v>9357</v>
       </c>
     </row>
@@ -6355,10 +6313,10 @@
       <c r="C22" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="D22" s="25">
+      <c r="D22" s="22">
         <v>450</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="22">
         <v>45</v>
       </c>
       <c r="F22" s="2">
@@ -6376,7 +6334,7 @@
       <c r="J22" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K22" s="26">
+      <c r="K22" s="23">
         <v>156</v>
       </c>
     </row>
@@ -6390,10 +6348,10 @@
       <c r="C23" s="2" t="s">
         <v>301</v>
       </c>
-      <c r="D23" s="25">
+      <c r="D23" s="22">
         <v>1045</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="22">
         <v>104.5</v>
       </c>
       <c r="F23" s="2">
@@ -6411,7 +6369,7 @@
       <c r="J23" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K23" s="26">
+      <c r="K23" s="23">
         <v>2579</v>
       </c>
     </row>
@@ -6425,10 +6383,10 @@
       <c r="C24" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D24" s="25">
+      <c r="D24" s="22">
         <v>2124.4699999999998</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="22">
         <v>212.45</v>
       </c>
       <c r="F24" s="2">
@@ -6446,7 +6404,7 @@
       <c r="J24" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="K24" s="26">
+      <c r="K24" s="23">
         <v>9357</v>
       </c>
     </row>
@@ -6460,10 +6418,10 @@
       <c r="C25" s="2" t="s">
         <v>320</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="22">
         <v>562.07000000000005</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="22">
         <v>56.21</v>
       </c>
       <c r="F25" s="2">
@@ -6481,7 +6439,7 @@
       <c r="J25" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K25" s="26">
+      <c r="K25" s="23">
         <v>156</v>
       </c>
     </row>
@@ -6495,10 +6453,10 @@
       <c r="C26" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="22">
         <v>637</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="22">
         <v>63.7</v>
       </c>
       <c r="F26" s="2">
@@ -6516,7 +6474,7 @@
       <c r="J26" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K26" s="26">
+      <c r="K26" s="23">
         <v>588</v>
       </c>
     </row>
@@ -6530,10 +6488,10 @@
       <c r="C27" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="D27" s="25">
+      <c r="D27" s="22">
         <v>268</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="22">
         <v>26.8</v>
       </c>
       <c r="F27" s="2">
@@ -6551,7 +6509,7 @@
       <c r="J27" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K27" s="26">
+      <c r="K27" s="23">
         <v>9865</v>
       </c>
     </row>
@@ -6565,10 +6523,10 @@
       <c r="C28" s="2" t="s">
         <v>323</v>
       </c>
-      <c r="D28" s="25">
+      <c r="D28" s="22">
         <v>1740.92</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="22">
         <v>174.09</v>
       </c>
       <c r="F28" s="2">
@@ -6586,7 +6544,7 @@
       <c r="J28" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K28" s="26">
+      <c r="K28" s="23">
         <v>156</v>
       </c>
     </row>
@@ -6600,10 +6558,10 @@
       <c r="C29" s="2" t="s">
         <v>324</v>
       </c>
-      <c r="D29" s="25">
+      <c r="D29" s="22">
         <v>8100</v>
       </c>
-      <c r="E29" s="25">
+      <c r="E29" s="22">
         <v>810</v>
       </c>
       <c r="F29" s="2">
@@ -6621,7 +6579,7 @@
       <c r="J29" s="2" t="s">
         <v>304</v>
       </c>
-      <c r="K29" s="26">
+      <c r="K29" s="23">
         <v>156</v>
       </c>
     </row>
@@ -6635,10 +6593,10 @@
       <c r="C30" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="D30" s="25">
+      <c r="D30" s="22">
         <v>600</v>
       </c>
-      <c r="E30" s="25">
+      <c r="E30" s="22">
         <v>60</v>
       </c>
       <c r="F30" s="2">
@@ -6656,7 +6614,7 @@
       <c r="J30" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K30" s="26">
+      <c r="K30" s="23">
         <v>588</v>
       </c>
     </row>
@@ -6670,10 +6628,10 @@
       <c r="C31" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="D31" s="25">
+      <c r="D31" s="22">
         <v>838.2</v>
       </c>
-      <c r="E31" s="25">
+      <c r="E31" s="22">
         <v>593.28</v>
       </c>
       <c r="F31" s="2">
@@ -6691,7 +6649,7 @@
       <c r="J31" s="2" t="s">
         <v>316</v>
       </c>
-      <c r="K31" s="26">
+      <c r="K31" s="23">
         <v>17470</v>
       </c>
     </row>
@@ -6705,10 +6663,10 @@
       <c r="C32" s="2" t="s">
         <v>326</v>
       </c>
-      <c r="D32" s="25">
+      <c r="D32" s="22">
         <v>838.2</v>
       </c>
-      <c r="E32" s="25">
+      <c r="E32" s="22">
         <v>593.28</v>
       </c>
       <c r="F32" s="2">
@@ -6726,7 +6684,7 @@
       <c r="J32" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K32" s="26">
+      <c r="K32" s="23">
         <v>9865</v>
       </c>
     </row>
@@ -6740,10 +6698,10 @@
       <c r="C33" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="D33" s="25">
+      <c r="D33" s="22">
         <v>1350</v>
       </c>
-      <c r="E33" s="25">
+      <c r="E33" s="22">
         <v>1056.52</v>
       </c>
       <c r="F33" s="2">
@@ -6761,7 +6719,7 @@
       <c r="J33" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K33" s="26">
+      <c r="K33" s="23">
         <v>9865</v>
       </c>
     </row>
@@ -6775,10 +6733,10 @@
       <c r="C34" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="D34" s="25">
+      <c r="D34" s="22">
         <v>2404</v>
       </c>
-      <c r="E34" s="25">
+      <c r="E34" s="22">
         <v>1935.22</v>
       </c>
       <c r="F34" s="2">
@@ -6796,7 +6754,7 @@
       <c r="J34" s="2" t="s">
         <v>297</v>
       </c>
-      <c r="K34" s="26">
+      <c r="K34" s="23">
         <v>9865</v>
       </c>
     </row>
@@ -6810,10 +6768,10 @@
       <c r="C35" s="2" t="s">
         <v>329</v>
       </c>
-      <c r="D35" s="25">
+      <c r="D35" s="22">
         <v>1089.5999999999999</v>
       </c>
-      <c r="E35" s="25">
+      <c r="E35" s="22">
         <v>1007.9</v>
       </c>
       <c r="F35" s="2">
@@ -6831,7 +6789,7 @@
       <c r="J35" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K35" s="26">
+      <c r="K35" s="23">
         <v>588</v>
       </c>
     </row>
@@ -6856,54 +6814,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>330</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>331</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>332</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>333</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="25" t="s">
         <v>334</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="26" t="s">
         <v>335</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="26" t="s">
         <v>336</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>337</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>338</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>339</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>340</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="24" t="s">
         <v>341</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>342</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="24" t="s">
         <v>343</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="24" t="s">
         <v>344</v>
       </c>
     </row>
@@ -6914,41 +6873,41 @@
       <c r="B2" s="2" t="s">
         <v>345</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="27">
         <v>45748</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31" t="s">
+      <c r="D2" s="28"/>
+      <c r="E2" s="28" t="s">
         <v>346</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="29">
         <v>20345</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="29">
         <v>2138</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="30" t="s">
         <v>348</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="30" t="s">
         <v>348</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>347</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="31" t="s">
         <v>349</v>
       </c>
     </row>
@@ -6979,25 +6938,24 @@
       <c r="B1" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="32" t="s">
         <v>351</v>
       </c>
-      <c r="E1" s="36">
-        <f>SUM(B2:B157)</f>
+      <c r="E1" s="33">
+        <v>15072</v>
+      </c>
+      <c r="F1" s="34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="35" t="s">
+        <v>290</v>
+      </c>
+      <c r="B2" s="36">
         <v>26</v>
       </c>
-      <c r="F1" s="37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
-        <v>290</v>
-      </c>
-      <c r="B2" s="39">
-        <v>26</v>
-      </c>
-      <c r="C2" s="37">
+      <c r="C2" s="34">
         <v>1.719349292421637E-3</v>
       </c>
     </row>

</xml_diff>